<commit_message>
Se agregaron Roles como R.H. e instructor
</commit_message>
<xml_diff>
--- a/Organización/Procesos/Soporte Organizacional/IWM_Matriz_de_ Roles.xlsx
+++ b/Organización/Procesos/Soporte Organizacional/IWM_Matriz_de_ Roles.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\IWM\CMMI3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gus\Documents\IWM\CMMI\GitHUB\Organización\Procesos\Soporte Organizacional\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="114">
   <si>
     <t>Nombre</t>
   </si>
@@ -335,9 +335,6 @@
     <t>Realizar la presentacion</t>
   </si>
   <si>
-    <t>duda</t>
-  </si>
-  <si>
     <t>Revisar avances en problemas anteriores</t>
   </si>
   <si>
@@ -345,6 +342,33 @@
   </si>
   <si>
     <t>Aprobar plan de capacitacion</t>
+  </si>
+  <si>
+    <t>Encargado de Recursos Humanos</t>
+  </si>
+  <si>
+    <t>Identificar Analisis de Capacitación</t>
+  </si>
+  <si>
+    <t>Elaborar plan de caparcitación</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implementacipon plan de capacitación </t>
+  </si>
+  <si>
+    <t>Actualizar plan de capacitación</t>
+  </si>
+  <si>
+    <t>Elaborar informe de resultados</t>
+  </si>
+  <si>
+    <t>Informar Resultados</t>
+  </si>
+  <si>
+    <t>Instructor</t>
+  </si>
+  <si>
+    <t>Implementar Capacitación</t>
   </si>
 </sst>
 </file>
@@ -744,7 +768,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="31">
+  <borders count="32">
     <border>
       <left/>
       <right/>
@@ -1090,6 +1114,19 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1139,7 +1176,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="45" applyFont="1"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="45" applyFont="1" applyAlignment="1">
@@ -1198,16 +1235,10 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="27" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="45" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="33" borderId="24" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="33" borderId="26" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="29" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1216,9 +1247,6 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="25" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="18" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="25" xfId="45" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="33" borderId="25" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1313,6 +1341,15 @@
     <xf numFmtId="0" fontId="0" fillId="26" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="26" xfId="45" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="27" xfId="45" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="15" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="31" xfId="45" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="21" xfId="45" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="46">
     <cellStyle name="20% - Accent1" xfId="1"/>
@@ -1660,8 +1697,8 @@
   </sheetPr>
   <dimension ref="A2:F122"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A85" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C67" sqref="C67"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A91" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C121" sqref="C121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -2146,7 +2183,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="43" t="s">
+      <c r="B5" s="40" t="s">
         <v>10</v>
       </c>
       <c r="C5" s="20" t="s">
@@ -2154,235 +2191,235 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="44"/>
+      <c r="B6" s="41"/>
       <c r="C6" s="21" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="44"/>
+      <c r="B7" s="41"/>
       <c r="C7" s="21" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="44"/>
+      <c r="B8" s="41"/>
       <c r="C8" s="21" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="44"/>
+      <c r="B9" s="41"/>
       <c r="C9" s="21" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="44"/>
+      <c r="B10" s="41"/>
       <c r="C10" s="21" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="44"/>
+      <c r="B11" s="41"/>
       <c r="C11" s="21" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="44"/>
+      <c r="B12" s="41"/>
       <c r="C12" s="21" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="44"/>
+      <c r="B13" s="41"/>
       <c r="C13" s="21" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="44"/>
+      <c r="B14" s="41"/>
       <c r="C14" s="21" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="44"/>
+      <c r="B15" s="41"/>
       <c r="C15" s="21" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="44"/>
+      <c r="B16" s="41"/>
       <c r="C16" s="21" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="17" spans="2:3" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="44"/>
+      <c r="B17" s="41"/>
       <c r="C17" s="21" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="18" spans="2:3" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="44"/>
+      <c r="B18" s="41"/>
       <c r="C18" s="21" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="19" spans="2:3" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="44"/>
+      <c r="B19" s="41"/>
       <c r="C19" s="21" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="20" spans="2:3" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="44"/>
+      <c r="B20" s="41"/>
       <c r="C20" s="21" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="21" spans="2:3" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="44"/>
+      <c r="B21" s="41"/>
       <c r="C21" s="21" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="22" spans="2:3" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="44"/>
+      <c r="B22" s="41"/>
       <c r="C22" s="21" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="23" spans="2:3" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="44"/>
+      <c r="B23" s="41"/>
       <c r="C23" s="21" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="24" spans="2:3" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="44"/>
+      <c r="B24" s="41"/>
       <c r="C24" s="21" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="25" spans="2:3" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="44"/>
+      <c r="B25" s="41"/>
       <c r="C25" s="21" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="26" spans="2:3" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="44"/>
+      <c r="B26" s="41"/>
       <c r="C26" s="21" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="27" spans="2:3" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="44"/>
+      <c r="B27" s="41"/>
       <c r="C27" s="21" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="28" spans="2:3" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="44"/>
+      <c r="B28" s="41"/>
       <c r="C28" s="21" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="29" spans="2:3" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="44"/>
+      <c r="B29" s="41"/>
       <c r="C29" s="21" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="30" spans="2:3" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="44"/>
+      <c r="B30" s="41"/>
       <c r="C30" s="21" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="31" spans="2:3" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B31" s="44"/>
+      <c r="B31" s="41"/>
       <c r="C31" s="21" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="32" spans="2:3" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B32" s="44"/>
+      <c r="B32" s="41"/>
       <c r="C32" s="21" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="33" spans="2:3" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="44"/>
+      <c r="B33" s="41"/>
       <c r="C33" s="21" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="34" spans="2:3" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B34" s="44"/>
+      <c r="B34" s="41"/>
       <c r="C34" s="21" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="35" spans="2:3" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B35" s="44"/>
+      <c r="B35" s="41"/>
       <c r="C35" s="21" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="36" spans="2:3" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B36" s="44"/>
+      <c r="B36" s="41"/>
       <c r="C36" s="21" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="37" spans="2:3" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B37" s="44"/>
+      <c r="B37" s="41"/>
       <c r="C37" s="21" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="38" spans="2:3" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B38" s="44"/>
+      <c r="B38" s="41"/>
       <c r="C38" s="21" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="39" spans="2:3" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B39" s="44"/>
+      <c r="B39" s="41"/>
       <c r="C39" s="21" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="40" spans="2:3" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B40" s="44"/>
+      <c r="B40" s="41"/>
       <c r="C40" s="21" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="41" spans="2:3" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B41" s="44"/>
+      <c r="B41" s="41"/>
       <c r="C41" s="21" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="42" spans="2:3" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B42" s="44"/>
+      <c r="B42" s="41"/>
       <c r="C42" s="21" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="43" spans="2:3" ht="14.25" customHeight="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="45"/>
+      <c r="B43" s="42"/>
       <c r="C43" s="22" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="44" spans="2:3" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B44" s="46" t="s">
+      <c r="B44" s="43" t="s">
         <v>12</v>
       </c>
       <c r="C44" s="23" t="s">
@@ -2390,67 +2427,67 @@
       </c>
     </row>
     <row r="45" spans="2:3" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B45" s="47"/>
+      <c r="B45" s="44"/>
       <c r="C45" s="24" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="46" spans="2:3" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B46" s="47"/>
+      <c r="B46" s="44"/>
       <c r="C46" s="24" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="47" spans="2:3" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B47" s="47"/>
+      <c r="B47" s="44"/>
       <c r="C47" s="24" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="48" spans="2:3" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B48" s="47"/>
+      <c r="B48" s="44"/>
       <c r="C48" s="24" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="49" spans="2:3" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B49" s="47"/>
+      <c r="B49" s="44"/>
       <c r="C49" s="24" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="50" spans="2:3" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B50" s="47"/>
+      <c r="B50" s="44"/>
       <c r="C50" s="24" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="51" spans="2:3" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B51" s="47"/>
+      <c r="B51" s="44"/>
       <c r="C51" s="24" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="52" spans="2:3" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B52" s="47"/>
+      <c r="B52" s="44"/>
       <c r="C52" s="24" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="53" spans="2:3" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B53" s="47"/>
+      <c r="B53" s="44"/>
       <c r="C53" s="24" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="54" spans="2:3" ht="15" customHeight="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="48"/>
+      <c r="B54" s="45"/>
       <c r="C54" s="25" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="55" spans="2:3" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B55" s="43" t="s">
+      <c r="B55" s="40" t="s">
         <v>16</v>
       </c>
       <c r="C55" s="20" t="s">
@@ -2458,49 +2495,49 @@
       </c>
     </row>
     <row r="56" spans="2:3" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B56" s="44"/>
+      <c r="B56" s="41"/>
       <c r="C56" s="21" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="57" spans="2:3" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B57" s="44"/>
+      <c r="B57" s="41"/>
       <c r="C57" s="21" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="58" spans="2:3" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B58" s="44"/>
+      <c r="B58" s="41"/>
       <c r="C58" s="26" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="59" spans="2:3" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B59" s="44"/>
+      <c r="B59" s="41"/>
       <c r="C59" s="26" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="60" spans="2:3" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B60" s="44"/>
+      <c r="B60" s="41"/>
       <c r="C60" s="26" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="61" spans="2:3" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B61" s="44"/>
+      <c r="B61" s="41"/>
       <c r="C61" s="26" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="62" spans="2:3" ht="15" customHeight="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="45"/>
+      <c r="B62" s="42"/>
       <c r="C62" s="27" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="63" spans="2:3" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B63" s="46" t="s">
+      <c r="B63" s="43" t="s">
         <v>15</v>
       </c>
       <c r="C63" s="28" t="s">
@@ -2508,63 +2545,63 @@
       </c>
     </row>
     <row r="64" spans="2:3" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B64" s="47"/>
+      <c r="B64" s="44"/>
       <c r="C64" s="24" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="65" spans="2:3" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B65" s="47"/>
+      <c r="B65" s="44"/>
       <c r="C65" s="24" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="66" spans="2:3" ht="15" customHeight="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="48"/>
+      <c r="B66" s="45"/>
       <c r="C66" s="25" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="67" spans="2:3" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B67" s="43" t="s">
+      <c r="B67" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="C67" s="31" t="s">
+      <c r="C67" s="30" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="68" spans="2:3" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B68" s="44"/>
-      <c r="C68" s="32" t="s">
+      <c r="B68" s="41"/>
+      <c r="C68" s="31" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="69" spans="2:3" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B69" s="44"/>
-      <c r="C69" s="32" t="s">
+      <c r="B69" s="41"/>
+      <c r="C69" s="31" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="70" spans="2:3" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B70" s="44"/>
+      <c r="B70" s="41"/>
       <c r="C70" s="26" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="71" spans="2:3" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B71" s="44"/>
+      <c r="B71" s="41"/>
       <c r="C71" s="26" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="72" spans="2:3" ht="15" customHeight="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B72" s="45"/>
+      <c r="B72" s="42"/>
       <c r="C72" s="27" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="73" spans="2:3" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B73" s="46" t="s">
+      <c r="B73" s="43" t="s">
         <v>13</v>
       </c>
       <c r="C73" s="23" t="s">
@@ -2572,162 +2609,159 @@
       </c>
     </row>
     <row r="74" spans="2:3" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B74" s="47"/>
+      <c r="B74" s="44"/>
       <c r="C74" s="24" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="75" spans="2:3" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B75" s="47"/>
+      <c r="B75" s="44"/>
       <c r="C75" s="24" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="76" spans="2:3" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B76" s="47"/>
+      <c r="B76" s="44"/>
       <c r="C76" s="24" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="77" spans="2:3" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B77" s="47"/>
+      <c r="B77" s="44"/>
       <c r="C77" s="24" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="78" spans="2:3" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B78" s="47"/>
+      <c r="B78" s="44"/>
       <c r="C78" s="24" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="79" spans="2:3" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B79" s="47"/>
+      <c r="B79" s="44"/>
       <c r="C79" s="24" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="80" spans="2:3" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B80" s="47"/>
+      <c r="B80" s="44"/>
       <c r="C80" s="24" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="81" spans="2:4" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B81" s="47"/>
+    <row r="81" spans="2:3" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B81" s="44"/>
       <c r="C81" s="24" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="82" spans="2:4" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B82" s="47"/>
+    <row r="82" spans="2:3" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B82" s="44"/>
       <c r="C82" s="24" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="83" spans="2:4" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B83" s="47"/>
+    <row r="83" spans="2:3" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B83" s="44"/>
       <c r="C83" s="24" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="84" spans="2:4" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B84" s="47"/>
+    <row r="84" spans="2:3" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B84" s="44"/>
       <c r="C84" s="24" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="85" spans="2:4" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B85" s="47"/>
+    <row r="85" spans="2:3" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B85" s="44"/>
       <c r="C85" s="24" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="86" spans="2:4" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B86" s="47"/>
+    <row r="86" spans="2:3" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B86" s="44"/>
       <c r="C86" s="24" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="87" spans="2:4" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B87" s="47"/>
+    <row r="87" spans="2:3" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B87" s="44"/>
       <c r="C87" s="24" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="88" spans="2:4" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B88" s="47"/>
+    <row r="88" spans="2:3" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B88" s="44"/>
       <c r="C88" s="24" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="89" spans="2:4" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B89" s="47"/>
+    <row r="89" spans="2:3" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B89" s="44"/>
       <c r="C89" s="24" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="90" spans="2:4" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B90" s="47"/>
+    <row r="90" spans="2:3" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B90" s="44"/>
       <c r="C90" s="24" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="91" spans="2:4" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B91" s="47"/>
+    <row r="91" spans="2:3" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B91" s="44"/>
       <c r="C91" s="24" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="92" spans="2:4" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B92" s="47"/>
+    <row r="92" spans="2:3" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B92" s="44"/>
       <c r="C92" s="24" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="93" spans="2:4" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B93" s="47"/>
+    <row r="93" spans="2:3" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B93" s="44"/>
       <c r="C93" s="24" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="94" spans="2:4" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B94" s="47"/>
-      <c r="C94" s="42" t="s">
+    <row r="94" spans="2:3" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B94" s="44"/>
+      <c r="C94" s="39" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="95" spans="2:4" ht="15" customHeight="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B95" s="48"/>
+    <row r="95" spans="2:3" ht="15" customHeight="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B95" s="45"/>
       <c r="C95" s="29" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="96" spans="2:4" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B96" s="43" t="s">
+    <row r="96" spans="2:3" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B96" s="40" t="s">
         <v>57</v>
       </c>
-      <c r="C96" s="31" t="s">
+      <c r="C96" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="D96" s="1" t="s">
-        <v>102</v>
-      </c>
     </row>
     <row r="97" spans="2:3" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B97" s="44"/>
-      <c r="C97" s="40" t="s">
+      <c r="B97" s="41"/>
+      <c r="C97" s="37" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="98" spans="2:3" ht="15" customHeight="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B98" s="45"/>
-      <c r="C98" s="41" t="s">
+      <c r="B98" s="42"/>
+      <c r="C98" s="38" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="99" spans="2:3" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B99" s="46" t="s">
+      <c r="B99" s="43" t="s">
         <v>76</v>
       </c>
       <c r="C99" s="28" t="s">
@@ -2735,90 +2769,127 @@
       </c>
     </row>
     <row r="100" spans="2:3" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B100" s="47"/>
-      <c r="C100" s="37" t="s">
+      <c r="B100" s="44"/>
+      <c r="C100" s="35" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="101" spans="2:3" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B101" s="47"/>
-      <c r="C101" s="37" t="s">
+      <c r="B101" s="44"/>
+      <c r="C101" s="35" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="102" spans="2:3" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B102" s="47"/>
-      <c r="C102" s="37" t="s">
+      <c r="B102" s="44"/>
+      <c r="C102" s="35" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="103" spans="2:3" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B103" s="47"/>
-      <c r="C103" s="37" t="s">
+      <c r="B103" s="44"/>
+      <c r="C103" s="35" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="104" spans="2:3" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B104" s="44"/>
+      <c r="C104" s="36" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="105" spans="2:3" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B105" s="44"/>
+      <c r="C105" s="36" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="106" spans="2:3" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B106" s="44"/>
+      <c r="C106" s="36" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="104" spans="2:3" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B104" s="47"/>
-      <c r="C104" s="39" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="105" spans="2:3" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B105" s="47"/>
-      <c r="C105" s="39" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="106" spans="2:3" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B106" s="47"/>
-      <c r="C106" s="39" t="s">
+    <row r="107" spans="2:3" ht="15" customHeight="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B107" s="44"/>
+      <c r="C107" s="36" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="107" spans="2:3" ht="15" customHeight="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B107" s="47"/>
-      <c r="C107" s="39" t="s">
-        <v>105</v>
-      </c>
-    </row>
     <row r="108" spans="2:3" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B108" s="46" t="s">
+      <c r="B108" s="40" t="s">
         <v>72</v>
       </c>
-      <c r="C108" s="28" t="s">
+      <c r="C108" s="30" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="109" spans="2:3" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B109" s="47"/>
+      <c r="B109" s="41"/>
       <c r="C109" s="37" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="110" spans="2:3" ht="15" customHeight="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B110" s="48"/>
-      <c r="C110" s="38" t="s">
+      <c r="B110" s="41"/>
+      <c r="C110" s="70" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="111" spans="2:3" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="B111" s="30"/>
-      <c r="C111" s="33"/>
-    </row>
-    <row r="112" spans="2:3" outlineLevel="1" x14ac:dyDescent="0.2"/>
-    <row r="113" outlineLevel="1" x14ac:dyDescent="0.2"/>
-    <row r="114" outlineLevel="1" x14ac:dyDescent="0.2"/>
-    <row r="115" outlineLevel="1" x14ac:dyDescent="0.2"/>
-    <row r="116" outlineLevel="1" x14ac:dyDescent="0.2"/>
-    <row r="117" outlineLevel="1" x14ac:dyDescent="0.2"/>
-    <row r="118" outlineLevel="1" x14ac:dyDescent="0.2"/>
-    <row r="119" outlineLevel="1" x14ac:dyDescent="0.2"/>
-    <row r="120" outlineLevel="1" x14ac:dyDescent="0.2"/>
-    <row r="121" outlineLevel="1" x14ac:dyDescent="0.2"/>
-    <row r="122" outlineLevel="1" x14ac:dyDescent="0.2"/>
+      <c r="B111" s="43" t="s">
+        <v>105</v>
+      </c>
+      <c r="C111" s="28" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="112" spans="2:3" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B112" s="44"/>
+      <c r="C112" s="68" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="113" spans="2:3" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B113" s="44"/>
+      <c r="C113" s="68" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="114" spans="2:3" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B114" s="44"/>
+      <c r="C114" s="68" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="115" spans="2:3" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="B115" s="44"/>
+      <c r="C115" s="68" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="116" spans="2:3" ht="13.5" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B116" s="45"/>
+      <c r="C116" s="69" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="117" spans="2:3" ht="13.5" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B117" s="71" t="s">
+        <v>112</v>
+      </c>
+      <c r="C117" s="72" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="118" spans="2:3" outlineLevel="1" x14ac:dyDescent="0.2"/>
+    <row r="119" spans="2:3" outlineLevel="1" x14ac:dyDescent="0.2"/>
+    <row r="120" spans="2:3" outlineLevel="1" x14ac:dyDescent="0.2"/>
+    <row r="121" spans="2:3" outlineLevel="1" x14ac:dyDescent="0.2"/>
+    <row r="122" spans="2:3" outlineLevel="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="10">
+    <mergeCell ref="B111:B116"/>
     <mergeCell ref="B5:B43"/>
     <mergeCell ref="B44:B54"/>
     <mergeCell ref="B96:B98"/>
@@ -2861,39 +2932,39 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D3" s="51" t="s">
+      <c r="D3" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="51"/>
+      <c r="E3" s="48"/>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="52" t="s">
+      <c r="C4" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="54" t="s">
+      <c r="D4" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="52" t="s">
+      <c r="E4" s="49" t="s">
         <v>56</v>
       </c>
-      <c r="F4" s="56" t="s">
+      <c r="F4" s="53" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="2:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="35" t="s">
+      <c r="B5" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="53"/>
-      <c r="D5" s="55"/>
-      <c r="E5" s="53"/>
-      <c r="F5" s="57"/>
+      <c r="C5" s="50"/>
+      <c r="D5" s="52"/>
+      <c r="E5" s="50"/>
+      <c r="F5" s="54"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B6" s="58" t="s">
+      <c r="B6" s="55" t="s">
         <v>14</v>
       </c>
       <c r="C6" s="8" t="s">
@@ -2910,21 +2981,21 @@
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B7" s="59"/>
+      <c r="B7" s="56"/>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
       <c r="F7" s="5"/>
     </row>
     <row r="8" spans="2:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="60"/>
+      <c r="B8" s="57"/>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
       <c r="E8" s="7"/>
       <c r="F8" s="10"/>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B9" s="61" t="s">
+      <c r="B9" s="58" t="s">
         <v>11</v>
       </c>
       <c r="C9" s="4"/>
@@ -2935,21 +3006,21 @@
       <c r="F9" s="11"/>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B10" s="62"/>
+      <c r="B10" s="59"/>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
       <c r="F10" s="5"/>
     </row>
     <row r="11" spans="2:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="63"/>
+      <c r="B11" s="60"/>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
       <c r="F11" s="10"/>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B12" s="58" t="s">
+      <c r="B12" s="55" t="s">
         <v>12</v>
       </c>
       <c r="C12" s="8" t="s">
@@ -2964,21 +3035,21 @@
       <c r="F12" s="5"/>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B13" s="59"/>
+      <c r="B13" s="56"/>
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
       <c r="F13" s="5"/>
     </row>
     <row r="14" spans="2:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="60"/>
+      <c r="B14" s="57"/>
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
       <c r="E14" s="7"/>
       <c r="F14" s="10"/>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B15" s="61" t="s">
+      <c r="B15" s="58" t="s">
         <v>16</v>
       </c>
       <c r="C15" s="4"/>
@@ -2989,39 +3060,39 @@
       <c r="F15" s="11"/>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B16" s="62"/>
+      <c r="B16" s="59"/>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
       <c r="F16" s="5"/>
     </row>
     <row r="17" spans="2:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="63"/>
+      <c r="B17" s="60"/>
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
       <c r="E17" s="7"/>
       <c r="F17" s="10"/>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B18" s="59" t="s">
+      <c r="B18" s="56" t="s">
         <v>15</v>
       </c>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
-      <c r="E18" s="36" t="s">
+      <c r="E18" s="34" t="s">
         <v>15</v>
       </c>
       <c r="F18" s="5"/>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B19" s="59"/>
+      <c r="B19" s="56"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="5"/>
     </row>
     <row r="20" spans="2:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="60"/>
+      <c r="B20" s="57"/>
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
       <c r="E20" s="7"/>
@@ -3032,44 +3103,44 @@
       <c r="B25" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="C25" s="49"/>
-      <c r="D25" s="49"/>
-      <c r="E25" s="49"/>
-      <c r="F25" s="50"/>
+      <c r="C25" s="46"/>
+      <c r="D25" s="46"/>
+      <c r="E25" s="46"/>
+      <c r="F25" s="47"/>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B26" s="64" t="s">
+      <c r="B26" s="61" t="s">
         <v>13</v>
       </c>
-      <c r="C26" s="67" t="s">
+      <c r="C26" s="64" t="s">
         <v>13</v>
       </c>
-      <c r="D26" s="67" t="s">
+      <c r="D26" s="64" t="s">
         <v>13</v>
       </c>
-      <c r="E26" s="67" t="s">
+      <c r="E26" s="64" t="s">
         <v>13</v>
       </c>
-      <c r="F26" s="69" t="s">
+      <c r="F26" s="66" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B27" s="65"/>
-      <c r="C27" s="68"/>
-      <c r="D27" s="68"/>
-      <c r="E27" s="68"/>
-      <c r="F27" s="70"/>
+      <c r="B27" s="62"/>
+      <c r="C27" s="65"/>
+      <c r="D27" s="65"/>
+      <c r="E27" s="65"/>
+      <c r="F27" s="67"/>
     </row>
     <row r="28" spans="2:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="66"/>
+      <c r="B28" s="63"/>
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
       <c r="E28" s="7"/>
       <c r="F28" s="10"/>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B29" s="58" t="s">
+      <c r="B29" s="55" t="s">
         <v>14</v>
       </c>
       <c r="C29" s="8" t="s">
@@ -3086,45 +3157,45 @@
       </c>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B30" s="59"/>
+      <c r="B30" s="56"/>
       <c r="C30" s="6"/>
       <c r="D30" s="6"/>
       <c r="E30" s="6"/>
       <c r="F30" s="5"/>
     </row>
     <row r="31" spans="2:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="60"/>
+      <c r="B31" s="57"/>
       <c r="C31" s="7"/>
       <c r="D31" s="7"/>
       <c r="E31" s="7"/>
       <c r="F31" s="10"/>
     </row>
     <row r="32" spans="2:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B32" s="64" t="s">
+      <c r="B32" s="61" t="s">
         <v>57</v>
       </c>
-      <c r="C32" s="67" t="s">
+      <c r="C32" s="64" t="s">
         <v>57</v>
       </c>
-      <c r="D32" s="67" t="s">
+      <c r="D32" s="64" t="s">
         <v>57</v>
       </c>
-      <c r="E32" s="67" t="s">
+      <c r="E32" s="64" t="s">
         <v>57</v>
       </c>
-      <c r="F32" s="69" t="s">
+      <c r="F32" s="66" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B33" s="65"/>
-      <c r="C33" s="68"/>
-      <c r="D33" s="68"/>
-      <c r="E33" s="68"/>
-      <c r="F33" s="70"/>
+      <c r="B33" s="62"/>
+      <c r="C33" s="65"/>
+      <c r="D33" s="65"/>
+      <c r="E33" s="65"/>
+      <c r="F33" s="67"/>
     </row>
     <row r="34" spans="2:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="66"/>
+      <c r="B34" s="63"/>
       <c r="C34" s="7"/>
       <c r="D34" s="7"/>
       <c r="E34" s="7"/>

</xml_diff>